<commit_message>
✏️ Update variance analysis and items
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,78 +480,134 @@
         <v>395335.8924431989</v>
       </c>
       <c r="C2" t="n">
-        <v>115087.4005825093</v>
+        <v>115196.8512725545</v>
       </c>
       <c r="D2" t="n">
-        <v>510423.2930257083</v>
+        <v>510532.7437157534</v>
       </c>
       <c r="E2" t="n">
-        <v>23757.72404239513</v>
+        <v>28579.68403444847</v>
       </c>
       <c r="F2" t="n">
-        <v>534181.0170681034</v>
+        <v>539112.4277502019</v>
       </c>
       <c r="G2" t="n">
-        <v>-30670.13430375629</v>
+        <v>-31269.57633747661</v>
       </c>
       <c r="H2" t="n">
-        <v>503510.8827643471</v>
+        <v>507842.8514127253</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Costi</t>
+          <t>Costi totali</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>291825.0433</v>
       </c>
       <c r="C3" t="n">
-        <v>84954.05122645351</v>
+        <v>85034.84442781005</v>
       </c>
       <c r="D3" t="n">
-        <v>376779.0945264535</v>
+        <v>376859.8877278101</v>
       </c>
       <c r="E3" t="n">
-        <v>32547.25614229194</v>
+        <v>36128.07294093538</v>
       </c>
       <c r="F3" t="n">
-        <v>409326.3506687455</v>
+        <v>412987.9606687455</v>
       </c>
       <c r="G3" t="n">
-        <v>74328.30933125445</v>
+        <v>74105.82933125459</v>
       </c>
       <c r="H3" t="n">
-        <v>483654.6599999999</v>
+        <v>487093.79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>Costi MP</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>172660.4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>50311.48145071982</v>
+      </c>
+      <c r="D4" t="n">
+        <v>222971.8814507198</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-10154.18096037768</v>
+      </c>
+      <c r="F4" t="n">
+        <v>212817.7004903422</v>
+      </c>
+      <c r="G4" t="n">
+        <v>46692.60950965786</v>
+      </c>
+      <c r="H4" t="n">
+        <v>259510.31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Costi risorse</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>119164.6433</v>
+      </c>
+      <c r="C5" t="n">
+        <v>34723.36297709029</v>
+      </c>
+      <c r="D5" t="n">
+        <v>153888.0062770903</v>
+      </c>
+      <c r="E5" t="n">
+        <v>46282.25390131297</v>
+      </c>
+      <c r="F5" t="n">
+        <v>200170.2601784033</v>
+      </c>
+      <c r="G5" t="n">
+        <v>27413.21982159675</v>
+      </c>
+      <c r="H5" t="n">
+        <v>227583.48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
           <t>MOL</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B6" t="n">
         <v>103510.8491431989</v>
       </c>
-      <c r="C4" t="n">
-        <v>30133.34935605584</v>
-      </c>
-      <c r="D4" t="n">
-        <v>133644.1984992548</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-8789.532099896809</v>
-      </c>
-      <c r="F4" t="n">
-        <v>124854.666399358</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-104998.4436350107</v>
-      </c>
-      <c r="H4" t="n">
-        <v>19856.22276434721</v>
+      <c r="C6" t="n">
+        <v>30162.00684474444</v>
+      </c>
+      <c r="D6" t="n">
+        <v>133672.8559879434</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-7548.388906486914</v>
+      </c>
+      <c r="F6" t="n">
+        <v>126124.4670814564</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-105375.4056687312</v>
+      </c>
+      <c r="H6" t="n">
+        <v>20749.06141272525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>